<commit_message>
Middle of refactoring effort. Still broken but syncing so work progress is not lost
</commit_message>
<xml_diff>
--- a/ApiSetHeirarchy.xlsx
+++ b/ApiSetHeirarchy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\graygeol\source\repos\HttpWebTester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6575AD38-AE79-473B-9C3A-0B29C6A86882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B93D87-77F1-47BC-A5E9-413A8A74A8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD49C4C0-3D0D-4F18-B090-60891D1D546A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{FD49C4C0-3D0D-4F18-B090-60891D1D546A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
   <si>
     <t>AbbreviatedResponseObject</t>
   </si>
@@ -138,10 +138,13 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>Extensions</t>
-  </si>
-  <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +211,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -221,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -241,7 +250,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -353,7 +364,7 @@
     <tableColumn id="9" xr3:uid="{A8C6967C-75D9-4EF9-A869-CA6C9531F543}" name="Class"/>
     <tableColumn id="10" xr3:uid="{F516E8A3-E990-49F0-8A28-FAB22741E136}" name="Lowest" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{7958037B-FA60-4815-96B4-9DB729703AA8}" name="Engine" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{43EB891B-1171-4FC2-98E4-EED9C24A0E0B}" name="Extensions" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{43EB891B-1171-4FC2-98E4-EED9C24A0E0B}" name="Created" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -659,17 +670,17 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="7" width="4.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="27" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="16"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -707,7 +718,7 @@
         <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -722,13 +733,13 @@
       <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="18">
         <v>5</v>
       </c>
-      <c r="K2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="8"/>
+      <c r="K2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -746,13 +757,13 @@
       <c r="I3" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="18">
         <v>1</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="8"/>
+      <c r="K3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -770,11 +781,11 @@
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="18">
         <v>2</v>
       </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="8"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -789,11 +800,13 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="J5" s="8">
+      <c r="J5" s="18">
         <v>2</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="8"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -808,14 +821,13 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
-      <c r="I6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="8"/>
+      <c r="J6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="19"/>
+      <c r="L6" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -830,14 +842,13 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="8"/>
+      <c r="J7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="19"/>
+      <c r="L7" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -855,13 +866,15 @@
       <c r="I8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="18">
         <v>2</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="8"/>
+      <c r="K8" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -879,13 +892,13 @@
       <c r="I9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="18">
         <v>2</v>
       </c>
-      <c r="K9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="8"/>
+      <c r="K9" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="18"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -903,13 +916,13 @@
       <c r="I10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="18">
         <v>3</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="8"/>
+      <c r="K10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -927,11 +940,13 @@
       <c r="I11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="18">
         <v>4</v>
       </c>
-      <c r="K11" s="17"/>
-      <c r="L11" s="8"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -949,11 +964,13 @@
       <c r="I12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="18">
         <v>7</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="8"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -971,11 +988,11 @@
       <c r="I13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="18">
         <v>4</v>
       </c>
-      <c r="K13" s="17"/>
-      <c r="L13" s="8"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="18"/>
     </row>
     <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -993,11 +1010,11 @@
       <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J14" s="18">
         <v>3</v>
       </c>
-      <c r="K14" s="17"/>
-      <c r="L14" s="8"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1012,11 +1029,13 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="J15" s="8">
+      <c r="J15" s="18">
         <v>5</v>
       </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="8"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1031,11 +1050,14 @@
       <c r="F16" s="12"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="J16" s="8">
+      <c r="I16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="18">
         <v>5</v>
       </c>
-      <c r="K16" s="17"/>
-      <c r="L16" s="8"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1053,13 +1075,15 @@
       <c r="I17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="8">
+      <c r="J17" s="18">
         <v>3</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L17" s="8"/>
+      <c r="K17" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1077,13 +1101,15 @@
       <c r="I18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="8">
+      <c r="J18" s="18">
         <v>4</v>
       </c>
-      <c r="K18" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="8"/>
+      <c r="K18" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1098,11 +1124,16 @@
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="J19" s="8">
+      <c r="I19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="17"/>
-      <c r="L19" s="8"/>
+      <c r="J19" s="18">
+        <v>6</v>
+      </c>
+      <c r="K19" s="19"/>
+      <c r="L19" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1117,11 +1148,16 @@
         <v>5</v>
       </c>
       <c r="H20" s="14"/>
-      <c r="J20" s="8">
+      <c r="I20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="18">
         <v>7</v>
       </c>
-      <c r="K20" s="17"/>
-      <c r="L20" s="8"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1136,11 +1172,16 @@
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
-      <c r="J21" s="8">
+      <c r="I21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K21" s="17"/>
-      <c r="L21" s="8"/>
+      <c r="J21" s="18">
+        <v>6</v>
+      </c>
+      <c r="K21" s="19"/>
+      <c r="L21" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1155,11 +1196,16 @@
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
-      <c r="J22" s="8">
+      <c r="I22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="18">
         <v>7</v>
       </c>
-      <c r="K22" s="17"/>
-      <c r="L22" s="8"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1174,14 +1220,13 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="8"/>
+      <c r="J23" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="19"/>
+      <c r="L23" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="24" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1199,13 +1244,13 @@
       <c r="I24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J24" s="8">
+      <c r="J24" s="18">
         <v>2</v>
       </c>
-      <c r="K24" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="L24" s="8"/>
+      <c r="K24" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" s="18"/>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -1220,11 +1265,16 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="7"/>
-      <c r="J25" s="8">
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="18">
         <v>5</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="8"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -1239,11 +1289,16 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="6"/>
-      <c r="J26" s="8">
+      <c r="I26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="8"/>
+      <c r="J26" s="18">
+        <v>6</v>
+      </c>
+      <c r="K26" s="19"/>
+      <c r="L26" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -1258,11 +1313,16 @@
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="5"/>
-      <c r="J27" s="8">
+      <c r="I27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="18">
         <v>7</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="8"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -1277,14 +1337,13 @@
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="8"/>
+      <c r="J28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="19"/>
+      <c r="L28" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -1302,11 +1361,11 @@
       <c r="I29" t="s">
         <v>2</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="18">
         <v>1</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="8"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="18"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -1324,11 +1383,13 @@
       <c r="I30" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="8"/>
+      <c r="J30" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="19"/>
+      <c r="L30" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -1343,11 +1404,13 @@
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-      <c r="J31" s="8">
+      <c r="J31" s="18">
         <v>2</v>
       </c>
-      <c r="K31" s="17"/>
-      <c r="L31" s="8"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
@@ -1365,11 +1428,11 @@
       <c r="I32" t="s">
         <v>7</v>
       </c>
-      <c r="J32" s="8">
+      <c r="J32" s="18">
         <v>1</v>
       </c>
-      <c r="K32" s="17"/>
-      <c r="L32" s="8"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="18"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1384,14 +1447,13 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
-      <c r="I33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K33" s="17"/>
-      <c r="L33" s="8"/>
+      <c r="J33" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="K33" s="19"/>
+      <c r="L33" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -1406,11 +1468,16 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="J34" s="8">
+      <c r="I34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K34" s="17"/>
-      <c r="L34" s="8"/>
+      <c r="J34" s="18">
+        <v>6</v>
+      </c>
+      <c r="K34" s="19"/>
+      <c r="L34" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1425,11 +1492,16 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
-      <c r="J35" s="8">
+      <c r="I35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="18">
         <v>7</v>
       </c>
-      <c r="K35" s="17"/>
-      <c r="L35" s="8"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>

</xml_diff>